<commit_message>
Adds un-archiving and copying functionality. Still should be finalized.
</commit_message>
<xml_diff>
--- a/download_request_example.xlsx
+++ b/download_request_example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MounSinai\Darpa\Programming\Sequence_results_downloader\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBAA401F-98AA-40CF-9BBA-413B91A5F8DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79318367-12F9-419B-8F5F-A384E9B2F8B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31875" yWindow="7320" windowWidth="22065" windowHeight="8370" xr2:uid="{101A21B5-97DD-4BA9-BCE4-FEC6819D6B6D}"/>
+    <workbookView xWindow="30795" yWindow="6150" windowWidth="25125" windowHeight="9210" xr2:uid="{101A21B5-97DD-4BA9-BCE4-FEC6819D6B6D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -46,32 +46,40 @@
     <t>Box</t>
   </si>
   <si>
-    <t>{box_mount_point}/methylation</t>
-  </si>
-  <si>
     <t>download_source</t>
   </si>
   <si>
     <t>destination</t>
   </si>
   <si>
-    <t>destination_directory_path</t>
-  </si>
-  <si>
     <t>unarchive_downloaded</t>
   </si>
   <si>
-    <t>yes</t>
+    <t>{box}/methylation</t>
+  </si>
+  <si>
+    <t>destination_path</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -94,13 +102,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -416,7 +427,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -430,40 +441,43 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
         <v>6</v>
-      </c>
-      <c r="D1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E2" t="s">
         <v>9</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{9128B7D2-1D07-4C99-B69C-167AC34E67EA}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>